<commit_message>
Added voice message support with Whisper and updated knowledge base
</commit_message>
<xml_diff>
--- a/RAG_knowledge_base_template.xlsx
+++ b/RAG_knowledge_base_template.xlsx
@@ -8,25 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projeckt\potokCash\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29739CB2-0CEE-474D-955A-C183B0BB6CF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E782B474-5D30-42C1-9CA5-AF8A0B4AFB80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About_Project" sheetId="1" r:id="rId1"/>
-    <sheet name="Income_Streams" sheetId="2" r:id="rId2"/>
-    <sheet name="Investment_Strategies" sheetId="3" r:id="rId3"/>
-    <sheet name="FAQ" sheetId="4" r:id="rId4"/>
-    <sheet name="Objections" sheetId="5" r:id="rId5"/>
-    <sheet name="Advantages" sheetId="6" r:id="rId6"/>
-    <sheet name="Crypto_Info" sheetId="7" r:id="rId7"/>
+    <sheet name="AML Policy" sheetId="8" r:id="rId2"/>
+    <sheet name="Income_Streams" sheetId="2" r:id="rId3"/>
+    <sheet name="Investment_Strategies" sheetId="3" r:id="rId4"/>
+    <sheet name="FAQ" sheetId="4" r:id="rId5"/>
+    <sheet name="Objections" sheetId="5" r:id="rId6"/>
+    <sheet name="Advantages" sheetId="6" r:id="rId7"/>
+    <sheet name="Crypto_Info" sheetId="7" r:id="rId8"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="233">
   <si>
     <t>Question_or_Title</t>
   </si>
@@ -677,13 +678,146 @@
     <t xml:space="preserve">Кто такой Васадин </t>
   </si>
   <si>
-    <t>Основатель — Васадин. Зачем создал: чтобы дать людям возможность достичь финансовой независимости без эксплуатации. Намерение: проект создан не для личного обогащения, а как "Народный Банк" с прозрачными алгоритмами.</t>
-  </si>
-  <si>
-    <t>Основатель — Васадин. Зачем создал: чтобы дать людям возможность достичь финансовой независимости без эксплуатации. Намерение: проект создан не для личного обогащения, а как "Народный Банк" с прозрачными алгоритмами. Его телеграм канал - https://t.me/kodvasadin</t>
-  </si>
-  <si>
     <t>Кто основатель</t>
+  </si>
+  <si>
+    <t>Основатель — Васадин. Зачем создал: чтобы дать людям возможность достичь финансовой независимости без эксплуатации. Намерение: проект создан не для личного обогащения, а как "Фонд народного обеспечения" и если сказать проще это как народный банк прозрачными алгоритмами. Его телеграм канал - https://t.me/kodvasadin</t>
+  </si>
+  <si>
+    <t>Основатель — Васадин. Зачем создал: чтобы дать людям возможность достичь финансовой независимости без эксплуатации. Намерение: проект создан не для личного обогащения, а как "Фонд народного обеспечения" и если сказать проще это как народный банк прозрачными алгоритмами.</t>
+  </si>
+  <si>
+    <t>Правила Проекта</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Соглашение о соблюдении правил Системы взаимной финансовой поддержки ПотокCash.Залогом успешной работы Системы является неукоснительное соблюдение правил всеми участниками.
+Эти правила очень простые и вам будет несложно их соблюдать, тем более, что если вдруг в процессе у вас возникнут какие-либо трудности, вы всегда сможете обратиться за помощью к своему Лидеру.
+</t>
+  </si>
+  <si>
+    <t>Что такое AML-политика проекта ПотокCash?</t>
+  </si>
+  <si>
+    <t>AML-политика — это меры по борьбе с отмыванием денег и финансированием терроризма. Она включает в себя мониторинг транзакций, проверку происхождения средств и личностей пользователей, чтобы предотвратить участие в незаконной деятельности.</t>
+  </si>
+  <si>
+    <t>Что такое KYC-политика?</t>
+  </si>
+  <si>
+    <t>KYC (Know Your Customer) — «Знай своего клиента» — политика, требующая от сервиса удостоверяться в личности клиента, источнике его средств и цели транзакций.</t>
+  </si>
+  <si>
+    <t>Кто проводит AML/KYC-проверки?</t>
+  </si>
+  <si>
+    <t>Проверки проводятся AML-офицером сервиса, а также автоматизированными криптоаналитическими системами, отслеживающими транзакции и происхождение активов.</t>
+  </si>
+  <si>
+    <t>Что происходит при подозрительной активности?</t>
+  </si>
+  <si>
+    <t>Если транзакция вызвала подозрение (например, пришла с чёрной площадки), она может быть заморожена до прохождения полной KYC-проверки.</t>
+  </si>
+  <si>
+    <t>Какие платформы находятся в чёрном списке?</t>
+  </si>
+  <si>
+    <t>Tornado Cash, Hydra, Garantex, Bitpapa, NetEx24, Grinex, Rapira.net, EMCD, и другие санкционные или нелегальные ресурсы.</t>
+  </si>
+  <si>
+    <t>Что будет, если активы пришли с запрещённой платформы?</t>
+  </si>
+  <si>
+    <t>Такие активы блокируются, и возврат средств невозможен. Пользователь должен пройти проверку, но средства, поступившие с санкционных источников, не подлежат возврату.</t>
+  </si>
+  <si>
+    <t>Что означает «высокий риск» транзакции?</t>
+  </si>
+  <si>
+    <t>Если по анализу активов получены метки вроде SCAM, MIXER, TERRORISM, FRAUD и т.д., активы могут быть заморожены до полной верификации или навсегда.</t>
+  </si>
+  <si>
+    <t>Какие страны запрещены для регистрации?</t>
+  </si>
+  <si>
+    <t>Проект не принимает клиентов из США, Ирана, КНДР, Сирии, Афганистана, Судана, Йемена, Венесуэлы и других стран, указанных в списке запрещённых юрисдикций.</t>
+  </si>
+  <si>
+    <t>Какие документы нужны для прохождения KYC?</t>
+  </si>
+  <si>
+    <t>Паспорт / ID-карта / водительское удостоверение, селфи с документом и листом с датой и подписью, подтверждение происхождения средств и переписка с отправителем.</t>
+  </si>
+  <si>
+    <t>Как подтвердить происхождение средств?</t>
+  </si>
+  <si>
+    <t>Нужно предоставить: историю переводов с платформы или кошелька-отправителя (скрины и ссылки на транзакции), объяснение за что были получены средства (услуга, работа и т.п.), контакт с отправителем и переписку, подтверждающую отправку.</t>
+  </si>
+  <si>
+    <t>Сколько времени занимает проверка?</t>
+  </si>
+  <si>
+    <t>Сроки рассмотрения документов индивидуальны и не регламентируются. Сервис может запросить дополнительные документы в любое время.</t>
+  </si>
+  <si>
+    <t>Что будет после успешного прохождения KYC?</t>
+  </si>
+  <si>
+    <t>Если проверка прошла успешно, активы возвращаются клиенту с удержанием комиссии 10%.</t>
+  </si>
+  <si>
+    <t>Когда возврат активов невозможен?</t>
+  </si>
+  <si>
+    <t>Если по активам был получен служебный запрос от поставщика ликвидности или компетентных органов, возврат невозможен — актив считается вещественным доказательством.</t>
+  </si>
+  <si>
+    <t>Кто такой AML-офицер?</t>
+  </si>
+  <si>
+    <t>Это назначенное ответственное лицо, которое следит за выполнением правил по борьбе с отмыванием денег, проводит проверки, мониторит активность и сотрудничает с регулирующими органами.</t>
+  </si>
+  <si>
+    <t>Что делает сервис для соблюдения AML/KYC?</t>
+  </si>
+  <si>
+    <t>Проводит постоянный мониторинг транзакций, использует риск-ориентированный подход, проверяет клиентов, назначает AML-офицера, взаимодействует с органами власти по запросу.</t>
+  </si>
+  <si>
+    <t>Какова основная суть правил проекта ПотокCash?</t>
+  </si>
+  <si>
+    <t>Суть правил — в поддержании честности, активности и личной ответственности каждого участника. Участник — это не потребитель, а совладелец проекта, который влияет на его развитие и успех.</t>
+  </si>
+  <si>
+    <t>Какие 6 правил участника ПотокCash?</t>
+  </si>
+  <si>
+    <t>Понимаю, что становлюсь совладельцем проекта.
+Заинтересован в развитии проекта и готов прилагать усилия.
+Готов распространять достоверную информацию о проекте.
+Поддерживаю уровень потока и использую возможности системы.
+Готов постоянно учиться и развиваться.
+Принимаю и поддерживаю изменения условий проекта.</t>
+  </si>
+  <si>
+    <t>Что будет, если участник нарушит правила проекта?</t>
+  </si>
+  <si>
+    <t>Если участник нарушает правила, распространяет негатив или действует нечестно, система может остановить начисления, обнулить поток и удалить аккаунт навсегда.</t>
+  </si>
+  <si>
+    <t>Можно ли иметь несколько аккаунтов?</t>
+  </si>
+  <si>
+    <t>Нет. Каждый участник имеет право на один личный аккаунт. Создание дополнительных — нарушение принципов честности и может привести к блокировке.</t>
+  </si>
+  <si>
+    <t>Что нужно делать для ежедневного получения награды?</t>
+  </si>
+  <si>
+    <t>Необходимо нажимать кнопку «Начислить награду» каждые 24 часа в Растущем и Быстром потоках.</t>
   </si>
 </sst>
 </file>
@@ -1113,10 +1247,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1149,7 +1283,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>187</v>
       </c>
@@ -1277,12 +1411,28 @@
         <v>184</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>188</v>
+    </row>
+    <row r="21" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>225</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>226</v>
       </c>
     </row>
   </sheetData>
@@ -1292,10 +1442,157 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{488CD7CA-6313-4782-8A17-A022745A431D}">
+  <dimension ref="A1:B16"/>
+  <sheetViews>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="46.28515625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="32.5703125" style="6" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>222</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -1382,12 +1679,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1433,12 +1730,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:B43"/>
+  <dimension ref="A1:B46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1791,18 +2088,42 @@
         <v>179</v>
       </c>
     </row>
+    <row r="44" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A44" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A45" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A46" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>232</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1864,12 +2185,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1982,17 +2303,25 @@
         <v>139</v>
       </c>
     </row>
+    <row r="14" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>228</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>